<commit_message>
Added the 'Driver', 'Toran' jobs, and removed the 'Fast caller and toran' job. Adapted the jobs to the functions in the app such as: 1. Adding a new person 2. Remove a person didn't adapet the main generate function to generate tzevet conan
</commit_message>
<xml_diff>
--- a/justice_board.xlsx
+++ b/justice_board.xlsx
@@ -3,13 +3,15 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9228" yWindow="1092" windowWidth="12120" windowHeight="8460" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Manager" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Samba" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Makel Officer" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Makel Operator" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Makel Officer" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Makel Operator" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Manager" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Samba" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Toran" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Driver" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -19,13 +21,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -44,12 +51,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -78,12 +100,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -451,7 +476,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,106 +485,63 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Sum</t>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>3+4</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>יועד בוגנר</t>
+          <t>of</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>אפק בן סימון</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>שלי מועלם</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>הודיה צפדיה</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>תומר שניידר</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>עמית גריסרו</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>יובל אבידן</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -573,7 +555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,215 +564,63 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Sum</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Samba</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Fast caller and Toran</t>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>3+4</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>יואב שוומנטל</t>
+          <t>op</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
-      </c>
-      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>1</v>
-      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>אביב זיתוני</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>רוני שור</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>תומר ארליכמן</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>8</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>עדו בורנשטיין</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>8</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>לוטן תמרי</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>17</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>רוני בורט</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>16</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>דיאנה פלדמן</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>16</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>אמבר פרץ</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>16</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>רומי שוחט</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>16</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -804,7 +634,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -813,101 +643,41 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>3+4</t>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Sum</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>יועד בוגנר</t>
+          <t>ma</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E2" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>אפק בן סימון</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>שלי מועלם</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>10</v>
-      </c>
-      <c r="D4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E4" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>הודיה צפדיה</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" t="n">
-        <v>10</v>
-      </c>
-      <c r="E5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -921,7 +691,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -930,101 +700,155 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>3+4</t>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Sum</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>יואב שוומנטל</t>
+          <t>sa</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E2" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>אביב זיתוני</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>רוני שור</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>10</v>
-      </c>
-      <c r="D4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E4" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>עדו בורנשטיין</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" t="n">
-        <v>10</v>
-      </c>
-      <c r="E5" t="n">
-        <v>20</v>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Sum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>to</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Sum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dr</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>